<commit_message>
Updated for aesthetics and other tinkering
</commit_message>
<xml_diff>
--- a/OD analyses MGM .xlsx
+++ b/OD analyses MGM .xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maltenform/Box Sync/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maltenform/Documents/GitHub/datahack2020/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A95794F2-CACA-A74E-A070-571F5B00176B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BAFD659-5FAA-BA4A-824B-CD4156091B18}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3480" yWindow="460" windowWidth="35160" windowHeight="19080" xr2:uid="{B20E8EA9-8070-294E-BA2F-F77232EE72C7}"/>
+    <workbookView xWindow="-1180" yWindow="460" windowWidth="28120" windowHeight="17540" xr2:uid="{B20E8EA9-8070-294E-BA2F-F77232EE72C7}"/>
   </bookViews>
   <sheets>
     <sheet name="P-values and Odds Ratios" sheetId="3" r:id="rId1"/>
     <sheet name="Tables" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="224">
   <si>
     <t>&lt;0.001</t>
   </si>
@@ -689,6 +689,15 @@
   </si>
   <si>
     <t>% Narcan</t>
+  </si>
+  <si>
+    <t>&gt;</t>
+  </si>
+  <si>
+    <t>19 or less</t>
+  </si>
+  <si>
+    <t>60 or more</t>
   </si>
 </sst>
 </file>
@@ -1068,10 +1077,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B5BF016-F4E1-EC45-AF29-CD696D9E0353}">
-  <dimension ref="B3:N38"/>
+  <dimension ref="B3:N79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1830,6 +1839,340 @@
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
+    </row>
+    <row r="42" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F42" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C43" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G43" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H43" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="I43" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J43" t="s">
+        <v>11</v>
+      </c>
+      <c r="K43" t="s">
+        <v>26</v>
+      </c>
+      <c r="L43" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="44" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B44" t="s">
+        <v>222</v>
+      </c>
+      <c r="C44">
+        <v>96</v>
+      </c>
+      <c r="D44">
+        <v>10</v>
+      </c>
+      <c r="E44" s="3">
+        <f>D44/C44</f>
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="F44">
+        <v>104</v>
+      </c>
+      <c r="G44">
+        <v>9</v>
+      </c>
+      <c r="H44" s="3">
+        <f>G44/F44</f>
+        <v>8.6538461538461536E-2</v>
+      </c>
+      <c r="I44" t="str">
+        <f>CONCATENATE(TEXT(J44,"0.00")," (",TEXT(K44,"0.00"),"-",TEXT(L44,"0.00"),")")</f>
+        <v>0.81 (0.32-2.10)</v>
+      </c>
+      <c r="J44" s="1">
+        <f>H44/(1-H44)*(1-E44)/E44</f>
+        <v>0.81473684210526309</v>
+      </c>
+      <c r="K44" s="1">
+        <f>EXP(LN(J44)-1.96*SQRT((1/D44+1/(C44-D44)+1/G44+1/(F44-G44))))</f>
+        <v>0.31615518582266605</v>
+      </c>
+      <c r="L44" s="1">
+        <f>EXP(LN(J44)+1.96*SQRT(1/D44+1/(C44-D44)+1/G44+1/(F44-G44)))</f>
+        <v>2.0995895422572155</v>
+      </c>
+    </row>
+    <row r="45" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
+        <v>6</v>
+      </c>
+      <c r="C45">
+        <v>348</v>
+      </c>
+      <c r="D45">
+        <v>105</v>
+      </c>
+      <c r="E45" s="3">
+        <f>D45/C45</f>
+        <v>0.30172413793103448</v>
+      </c>
+      <c r="F45">
+        <v>724</v>
+      </c>
+      <c r="G45">
+        <v>30</v>
+      </c>
+      <c r="H45" s="3">
+        <f>G45/F45</f>
+        <v>4.1436464088397788E-2</v>
+      </c>
+      <c r="I45" t="str">
+        <f>CONCATENATE(TEXT(J45,"0.00")," (",TEXT(K45,"0.00"),"-",TEXT(L45,"0.00"),")")</f>
+        <v>0.10 (0.06-0.15)</v>
+      </c>
+      <c r="J45" s="1">
+        <f>H45/(1-H45)*(1-E45)/E45</f>
+        <v>0.10004116920543432</v>
+      </c>
+      <c r="K45" s="1">
+        <f>EXP(LN(J45)-1.96*SQRT((1/D45+1/(C45-D45)+1/G45+1/(F45-G45))))</f>
+        <v>6.4995795962699957E-2</v>
+      </c>
+      <c r="L45" s="1">
+        <f>EXP(LN(J45)+1.96*SQRT(1/D45+1/(C45-D45)+1/G45+1/(F45-G45)))</f>
+        <v>0.15398281362280583</v>
+      </c>
+    </row>
+    <row r="46" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B46" t="s">
+        <v>7</v>
+      </c>
+      <c r="C46">
+        <v>606</v>
+      </c>
+      <c r="D46">
+        <v>190</v>
+      </c>
+      <c r="E46" s="3">
+        <f t="shared" ref="E46:E47" si="2">D46/C46</f>
+        <v>0.31353135313531355</v>
+      </c>
+      <c r="F46">
+        <v>1338</v>
+      </c>
+      <c r="G46">
+        <v>76</v>
+      </c>
+      <c r="H46" s="3">
+        <f>G46/F46</f>
+        <v>5.6801195814648729E-2</v>
+      </c>
+      <c r="I46" t="str">
+        <f>CONCATENATE(TEXT(J46,"0.00")," (",TEXT(K46,"0.00"),"-",TEXT(L46,"0.00"),")")</f>
+        <v>0.13 (0.10-0.18)</v>
+      </c>
+      <c r="J46" s="1">
+        <f>H46/(1-H46)*(1-E46)/E46</f>
+        <v>0.13185419968304277</v>
+      </c>
+      <c r="K46" s="1">
+        <f>EXP(LN(J46)-1.96*SQRT((1/D46+1/(C46-D46)+1/G46+1/(F46-G46))))</f>
+        <v>9.884188882083933E-2</v>
+      </c>
+      <c r="L46" s="1">
+        <f>EXP(LN(J46)+1.96*SQRT(1/D46+1/(C46-D46)+1/G46+1/(F46-G46)))</f>
+        <v>0.17589232845973535</v>
+      </c>
+    </row>
+    <row r="47" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C47">
+        <v>989</v>
+      </c>
+      <c r="D47">
+        <v>354</v>
+      </c>
+      <c r="E47" s="3">
+        <f t="shared" si="2"/>
+        <v>0.35793731041456017</v>
+      </c>
+      <c r="F47">
+        <v>2109</v>
+      </c>
+      <c r="G47">
+        <v>148</v>
+      </c>
+      <c r="H47" s="3">
+        <f>G47/F47</f>
+        <v>7.0175438596491224E-2</v>
+      </c>
+      <c r="I47" t="str">
+        <f>CONCATENATE(TEXT(J47,"0.00")," (",TEXT(K47,"0.00"),"-",TEXT(L47,"0.00"),")")</f>
+        <v>0.14 (0.11-0.17)</v>
+      </c>
+      <c r="J47" s="1">
+        <f>H47/(1-H47)*(1-E47)/E47</f>
+        <v>0.13538002345165759</v>
+      </c>
+      <c r="K47" s="1">
+        <f>EXP(LN(J47)-1.96*SQRT((1/D47+1/(C47-D47)+1/G47+1/(F47-G47))))</f>
+        <v>0.10955036252579411</v>
+      </c>
+      <c r="L47" s="1">
+        <f>EXP(LN(J47)+1.96*SQRT(1/D47+1/(C47-D47)+1/G47+1/(F47-G47)))</f>
+        <v>0.16729977270003105</v>
+      </c>
+    </row>
+    <row r="48" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B48" t="s">
+        <v>9</v>
+      </c>
+      <c r="C48">
+        <v>467</v>
+      </c>
+      <c r="D48">
+        <v>203</v>
+      </c>
+      <c r="E48" s="3">
+        <f t="shared" ref="E48:E50" si="3">D48/C48</f>
+        <v>0.43468950749464669</v>
+      </c>
+      <c r="F48">
+        <v>793</v>
+      </c>
+      <c r="G48">
+        <v>69</v>
+      </c>
+      <c r="H48" s="3">
+        <f t="shared" ref="H48:H50" si="4">G48/F48</f>
+        <v>8.7011349306431271E-2</v>
+      </c>
+      <c r="I48" t="str">
+        <f t="shared" ref="I48:I50" si="5">CONCATENATE(TEXT(J48,"0.00")," (",TEXT(K48,"0.00"),"-",TEXT(L48,"0.00"),")")</f>
+        <v>0.12 (0.09-0.17)</v>
+      </c>
+      <c r="J48" s="1">
+        <f t="shared" ref="J48:J50" si="6">H48/(1-H48)*(1-E48)/E48</f>
+        <v>0.12394197534224206</v>
+      </c>
+      <c r="K48" s="1">
+        <f t="shared" ref="K48:K50" si="7">EXP(LN(J48)-1.96*SQRT((1/D48+1/(C48-D48)+1/G48+1/(F48-G48))))</f>
+        <v>9.1147109475755578E-2</v>
+      </c>
+      <c r="L48" s="1">
+        <f t="shared" ref="L48:L50" si="8">EXP(LN(J48)+1.96*SQRT(1/D48+1/(C48-D48)+1/G48+1/(F48-G48)))</f>
+        <v>0.16853648283627704</v>
+      </c>
+    </row>
+    <row r="49" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B49" t="s">
+        <v>10</v>
+      </c>
+      <c r="C49">
+        <v>269</v>
+      </c>
+      <c r="D49">
+        <v>131</v>
+      </c>
+      <c r="E49" s="3">
+        <f t="shared" si="3"/>
+        <v>0.48698884758364314</v>
+      </c>
+      <c r="F49">
+        <v>452</v>
+      </c>
+      <c r="G49">
+        <v>28</v>
+      </c>
+      <c r="H49" s="3">
+        <f t="shared" si="4"/>
+        <v>6.1946902654867256E-2</v>
+      </c>
+      <c r="I49" t="str">
+        <f t="shared" si="5"/>
+        <v>0.07 (0.04-0.11)</v>
+      </c>
+      <c r="J49" s="1">
+        <f t="shared" si="6"/>
+        <v>6.9566469825723745E-2</v>
+      </c>
+      <c r="K49" s="1">
+        <f t="shared" si="7"/>
+        <v>4.4312111184777722E-2</v>
+      </c>
+      <c r="L49" s="1">
+        <f t="shared" si="8"/>
+        <v>0.10921379267697393</v>
+      </c>
+    </row>
+    <row r="50" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B50" t="s">
+        <v>223</v>
+      </c>
+      <c r="C50">
+        <v>89</v>
+      </c>
+      <c r="D50">
+        <v>45</v>
+      </c>
+      <c r="E50" s="3">
+        <f t="shared" si="3"/>
+        <v>0.5056179775280899</v>
+      </c>
+      <c r="F50">
+        <v>141</v>
+      </c>
+      <c r="G50">
+        <v>7</v>
+      </c>
+      <c r="H50" s="3">
+        <f t="shared" si="4"/>
+        <v>4.9645390070921988E-2</v>
+      </c>
+      <c r="I50" t="str">
+        <f t="shared" si="5"/>
+        <v>0.05 (0.02-0.12)</v>
+      </c>
+      <c r="J50" s="1">
+        <f t="shared" si="6"/>
+        <v>5.107794361525704E-2</v>
+      </c>
+      <c r="K50" s="1">
+        <f t="shared" si="7"/>
+        <v>2.148258725675271E-2</v>
+      </c>
+      <c r="L50" s="1">
+        <f t="shared" si="8"/>
+        <v>0.12144516360073407</v>
+      </c>
+    </row>
+    <row r="79" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B79" t="s">
+        <v>221</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>